<commit_message>
changing assets - quality+low volatily
</commit_message>
<xml_diff>
--- a/input/assets.xlsx
+++ b/input/assets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Investments\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935cc860ba0efd68/GitHub/myportfolio/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10D7187-5546-4483-8DEF-63838578FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{B10D7187-5546-4483-8DEF-63838578FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B9E339D-7743-4C49-8537-FEFFAFEA1532}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -280,7 +280,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="211">
   <si>
     <t>iShares Core MSCI World UCITS ETF USD</t>
   </si>
@@ -1058,9 +1058,6 @@
     <t>Valuta indifferente nel lungo periodo. Meglio non hedgiati</t>
   </si>
   <si>
-    <t>Healthcare Global</t>
-  </si>
-  <si>
     <t>Small Cap Global</t>
   </si>
   <si>
@@ -1103,9 +1100,6 @@
     <t>Consumer Staples Global</t>
   </si>
   <si>
-    <t>Momentum Global</t>
-  </si>
-  <si>
     <t>Xtrackers MSCI World Consumer Staples UCITS ETF 1C | XDWS | IE00BM67HN09</t>
   </si>
   <si>
@@ -1182,6 +1176,60 @@
   </si>
   <si>
     <t>IE00BF4RFH31</t>
+  </si>
+  <si>
+    <t>IE00BP3QZ601</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI World Quality Factor UCITS ETF (Acc)</t>
+  </si>
+  <si>
+    <t>IWQU.L</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI World Minimum Volatility UCITS ETF USD (Acc)</t>
+  </si>
+  <si>
+    <t>IE00B8FHGS14</t>
+  </si>
+  <si>
+    <t>MVOL.L</t>
+  </si>
+  <si>
+    <t>low volatility</t>
+  </si>
+  <si>
+    <t>world quality</t>
+  </si>
+  <si>
+    <t>US quality</t>
+  </si>
+  <si>
+    <t>IE00BD1F4L37</t>
+  </si>
+  <si>
+    <t>QDVB.DE</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI USA Quality Factor UCITS ETF</t>
+  </si>
+  <si>
+    <t>World Momentum</t>
+  </si>
+  <si>
+    <t>US Quality</t>
+  </si>
+  <si>
+    <t>World Low Volatility</t>
+  </si>
+  <si>
+    <t>World Healthcare</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI USA Quality Factor UCITS ETF | QDVB | IE00BD1F4L37</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI World Minimum Volatility UCITS ETF USD (Acc) | MVOL | IE00B8FHGS14</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1665,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1670,6 +1718,187 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1679,190 +1908,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8"/>
@@ -2149,13 +2201,13 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="39.9453125" customWidth="1"/>
-    <col min="2" max="2" width="28.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7890625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.1015625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.41796875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="7.9453125" bestFit="1" customWidth="1"/>
@@ -2169,7 +2221,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>19</v>
@@ -2206,20 +2258,20 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="100" t="s">
-        <v>170</v>
+      <c r="A2" s="36" t="s">
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>205</v>
       </c>
       <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" t="s">
         <v>156</v>
       </c>
-      <c r="D2" t="s">
-        <v>157</v>
-      </c>
       <c r="E2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -2228,7 +2280,7 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I2" s="1">
         <v>2.5000000000000001E-3</v>
@@ -2244,20 +2296,20 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="100" t="s">
-        <v>169</v>
+      <c r="A3" s="36" t="s">
+        <v>209</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>204</v>
       </c>
       <c r="D3" t="s">
-        <v>162</v>
+        <v>202</v>
       </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>203</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -2266,30 +2318,30 @@
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>186</v>
+        <v>32</v>
       </c>
       <c r="I3" s="1">
-        <v>2.5000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="J3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="100" t="s">
-        <v>171</v>
+      <c r="A4" s="36" t="s">
+        <v>210</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" t="s">
-        <v>166</v>
+        <v>207</v>
+      </c>
+      <c r="C4" s="102" t="s">
+        <v>196</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>198</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -2298,30 +2350,30 @@
         <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>186</v>
+        <v>32</v>
       </c>
       <c r="I4" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="100" t="s">
-        <v>172</v>
+      <c r="A5" s="36" t="s">
+        <v>169</v>
       </c>
       <c r="B5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" t="s">
         <v>154</v>
-      </c>
-      <c r="C5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" t="s">
-        <v>194</v>
-      </c>
-      <c r="E5" t="s">
-        <v>159</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -2330,30 +2382,30 @@
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I5" s="1">
-        <v>3.5000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
         <v>173</v>
       </c>
-      <c r="B6" t="s">
-        <v>175</v>
-      </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -2362,7 +2414,7 @@
         <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I6" s="1">
         <v>1.5E-3</v>
@@ -2378,20 +2430,20 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" t="s">
         <v>177</v>
       </c>
-      <c r="B7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" t="s">
-        <v>179</v>
-      </c>
       <c r="E7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -2400,7 +2452,7 @@
         <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I7" s="1">
         <v>1E-3</v>
@@ -2416,20 +2468,20 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="100" t="s">
+      <c r="A8" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" t="s">
         <v>182</v>
       </c>
-      <c r="B8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>183</v>
-      </c>
-      <c r="D8" t="s">
-        <v>184</v>
-      </c>
-      <c r="E8" t="s">
-        <v>185</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -2438,7 +2490,7 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I8" s="1">
         <v>6.9999999999999999E-4</v>
@@ -2451,20 +2503,20 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="100" t="s">
-        <v>190</v>
+      <c r="A9" s="36" t="s">
+        <v>188</v>
       </c>
       <c r="B9" t="s">
         <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E9" t="s">
         <v>187</v>
-      </c>
-      <c r="E9" t="s">
-        <v>189</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
@@ -2473,7 +2525,7 @@
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I9" s="1">
         <v>1.1999999999999999E-3</v>
@@ -2490,14 +2542,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BM67HN09" xr:uid="{910EFAF6-3CEE-4CB8-8783-0CCFA8F4D835}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BP3QZ825" xr:uid="{5E561C16-8B8B-483B-AA10-D0DDAD2EE0FF}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BYTRRB94" xr:uid="{7F0259C1-E0BF-4DDA-8122-BE9F2BE69234}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BF4RFH31" xr:uid="{684559CE-9181-4573-92B0-6AF7C01E84D0}"/>
-    <hyperlink ref="A6" r:id="rId5" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B3VTN290" xr:uid="{6AB80B8F-0CAF-4297-B9BB-D72ED9AFBF01}"/>
-    <hyperlink ref="A8" r:id="rId6" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{69029A56-B54E-49FD-A0F5-77171229A26E}"/>
-    <hyperlink ref="A9" r:id="rId7" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B579F325" xr:uid="{42CB0A67-6EA5-4F8A-A191-29BAAE4A4956}"/>
-    <hyperlink ref="A7" r:id="rId8" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BDQYWQ65" xr:uid="{6C04B138-97D3-42C8-B6E1-00870CCBE0B4}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BP3QZ825" xr:uid="{5E561C16-8B8B-483B-AA10-D0DDAD2EE0FF}"/>
+    <hyperlink ref="A5" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BYTRRB94" xr:uid="{7F0259C1-E0BF-4DDA-8122-BE9F2BE69234}"/>
+    <hyperlink ref="A6" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B3VTN290" xr:uid="{6AB80B8F-0CAF-4297-B9BB-D72ED9AFBF01}"/>
+    <hyperlink ref="A8" r:id="rId4" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{69029A56-B54E-49FD-A0F5-77171229A26E}"/>
+    <hyperlink ref="A9" r:id="rId5" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B579F325" xr:uid="{42CB0A67-6EA5-4F8A-A191-29BAAE4A4956}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BDQYWQ65" xr:uid="{6C04B138-97D3-42C8-B6E1-00870CCBE0B4}"/>
+    <hyperlink ref="A3" r:id="rId7" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BD1F4L37" xr:uid="{DF84D7C7-B8F6-477A-8C9A-D4997B54C865}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B8FHGS14" xr:uid="{47A684AB-EAC0-4609-B6F5-2C135D16A87D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2878,297 +2930,453 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222E099E-8C0E-4FA4-8471-33732A50ACAC}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:H9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.9453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.68359375" customWidth="1"/>
+    <col min="3" max="3" width="52.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12">
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12">
+      <c r="B2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>74</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>73</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>72</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>54</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12">
+      <c r="B3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>66</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>2E-3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12">
+      <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>48</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>67</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>34</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12">
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>61</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>34</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
+    <row r="6" spans="1:12">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>68</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>1.5E-3</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>34</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
+    <row r="7" spans="1:12">
+      <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>65</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>34</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
+    <row r="8" spans="1:12">
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>62</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="1">
+      <c r="I8" s="1">
         <v>2E-3</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>34</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
+    <row r="9" spans="1:12">
+      <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>64</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="1">
+      <c r="I9" s="1">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="10" spans="1:12">
+      <c r="B10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="14.7" customHeight="1">
+      <c r="B11" t="s">
+        <v>199</v>
+      </c>
+      <c r="C11" s="101" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E11" t="s">
+        <v>198</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="B12" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E12" t="s">
+        <v>203</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" t="s">
+        <v>162</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" t="s">
+        <v>184</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" t="s">
+        <v>184</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A13" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BM67HN09" xr:uid="{910EFAF6-3CEE-4CB8-8783-0CCFA8F4D835}"/>
+    <hyperlink ref="A14" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BF4RFH31" xr:uid="{684559CE-9181-4573-92B0-6AF7C01E84D0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3196,31 +3404,31 @@
         <v>IWMO.L</v>
       </c>
       <c r="B2" t="str">
-        <v>Momentum Global</v>
+        <v>World Momentum</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="str">
-        <v>XDWS.L</v>
+        <v>QDVB.DE</v>
       </c>
       <c r="B3" t="str">
-        <v>Consumer Staples Global</v>
+        <v>US Quality</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="str">
-        <v>WHEA.L</v>
+        <v>MVOL.L</v>
       </c>
       <c r="B4" t="str">
-        <v>Healthcare Global</v>
+        <v>World Low Volatility</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="str">
-        <v>WSML.L</v>
+        <v>WHEA.L</v>
       </c>
       <c r="B5" t="str">
-        <v>Small Cap Global</v>
+        <v>World Healthcare</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3283,17 +3491,17 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="str">
-        <v>Xtrackers MSCI World Consumer Staples UCITS ETF (Acc)</v>
+        <v>iShares Edge MSCI USA Quality Factor UCITS ETF</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="str">
-        <v>SPDR MSCI World Health Care UCITS ETF</v>
+        <v>iShares Edge MSCI World Minimum Volatility UCITS ETF USD (Acc)</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="str">
-        <v>iShares MSCI World Small Cap UCITS ETF</v>
+        <v>SPDR MSCI World Health Care UCITS ETF</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -3341,118 +3549,118 @@
     </row>
     <row r="3" spans="1:18" ht="14.7" thickBot="1"/>
     <row r="4" spans="1:18" ht="16" customHeight="1">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
-      <c r="H4" s="94" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="39"/>
+      <c r="H4" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="96"/>
-      <c r="N4" s="70" t="s">
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="45"/>
+      <c r="N4" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="O4" s="71"/>
-      <c r="P4" s="71"/>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="72"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="51"/>
     </row>
     <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="B5" s="61"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="63"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="99"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="75"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="48"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="54"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="51"/>
-      <c r="H6" s="49" t="s">
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="57"/>
+      <c r="H6" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="51"/>
-      <c r="N6" s="49" t="s">
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="57"/>
+      <c r="N6" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="51"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="57"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="B7" s="52"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="54"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="54"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="54"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="60"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="60"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="59"/>
+      <c r="R7" s="60"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="B8" s="52"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="54"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="54"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="53"/>
-      <c r="R8" s="54"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="60"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="59"/>
+      <c r="Q8" s="59"/>
+      <c r="R8" s="60"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="B9" s="55"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="57"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="57"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="56"/>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="57"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="63"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="63"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="63"/>
     </row>
     <row r="10" spans="1:18">
       <c r="B10" s="5"/>
@@ -3473,226 +3681,226 @@
     </row>
     <row r="11" spans="1:18" ht="14.7" thickBot="1"/>
     <row r="12" spans="1:18" ht="16" customHeight="1">
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="60"/>
-      <c r="H12" s="82" t="s">
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="39"/>
+      <c r="H12" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="I12" s="83"/>
-      <c r="J12" s="83"/>
-      <c r="K12" s="83"/>
-      <c r="L12" s="84"/>
-      <c r="N12" s="88" t="s">
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="66"/>
+      <c r="N12" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="O12" s="89"/>
-      <c r="P12" s="89"/>
-      <c r="Q12" s="89"/>
-      <c r="R12" s="90"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="71"/>
+      <c r="Q12" s="71"/>
+      <c r="R12" s="72"/>
     </row>
     <row r="13" spans="1:18" ht="16" customHeight="1">
-      <c r="B13" s="61"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="63"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
-      <c r="L13" s="87"/>
-      <c r="N13" s="91"/>
-      <c r="O13" s="92"/>
-      <c r="P13" s="92"/>
-      <c r="Q13" s="92"/>
-      <c r="R13" s="93"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="69"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="74"/>
+      <c r="P13" s="74"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="75"/>
     </row>
     <row r="14" spans="1:18" ht="16" customHeight="1">
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
-      <c r="H14" s="39" t="s">
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="78"/>
+      <c r="H14" s="76" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="41"/>
-      <c r="N14" s="39" t="s">
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="78"/>
+      <c r="N14" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="O14" s="40"/>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="41"/>
+      <c r="O14" s="77"/>
+      <c r="P14" s="77"/>
+      <c r="Q14" s="77"/>
+      <c r="R14" s="78"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="44"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="44"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="43"/>
-      <c r="R15" s="44"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="81"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="80"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="81"/>
+      <c r="N15" s="79"/>
+      <c r="O15" s="80"/>
+      <c r="P15" s="80"/>
+      <c r="Q15" s="80"/>
+      <c r="R15" s="81"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="44"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="43"/>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="44"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="81"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="81"/>
+      <c r="N16" s="79"/>
+      <c r="O16" s="80"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="81"/>
     </row>
     <row r="17" spans="2:18">
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="44"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="44"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="43"/>
-      <c r="R17" s="44"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="81"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="80"/>
+      <c r="L17" s="81"/>
+      <c r="N17" s="79"/>
+      <c r="O17" s="80"/>
+      <c r="P17" s="80"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="81"/>
     </row>
     <row r="18" spans="2:18">
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="47"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="47"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="84"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="83"/>
+      <c r="J18" s="83"/>
+      <c r="K18" s="83"/>
+      <c r="L18" s="84"/>
+      <c r="N18" s="82"/>
+      <c r="O18" s="83"/>
+      <c r="P18" s="83"/>
+      <c r="Q18" s="83"/>
+      <c r="R18" s="84"/>
     </row>
     <row r="19" spans="2:18" ht="16" customHeight="1">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="76" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
-      <c r="H19" s="39" t="s">
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="78"/>
+      <c r="H19" s="76" t="s">
         <v>106</v>
       </c>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="41"/>
-      <c r="N19" s="39" t="s">
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="77"/>
+      <c r="L19" s="78"/>
+      <c r="N19" s="76" t="s">
         <v>107</v>
       </c>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="41"/>
+      <c r="O19" s="77"/>
+      <c r="P19" s="77"/>
+      <c r="Q19" s="77"/>
+      <c r="R19" s="78"/>
     </row>
     <row r="20" spans="2:18">
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="44"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="44"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="43"/>
-      <c r="R20" s="44"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="81"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="80"/>
+      <c r="K20" s="80"/>
+      <c r="L20" s="81"/>
+      <c r="N20" s="79"/>
+      <c r="O20" s="80"/>
+      <c r="P20" s="80"/>
+      <c r="Q20" s="80"/>
+      <c r="R20" s="81"/>
     </row>
     <row r="21" spans="2:18">
-      <c r="B21" s="42"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="44"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="44"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="43"/>
-      <c r="R21" s="44"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="81"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="80"/>
+      <c r="K21" s="80"/>
+      <c r="L21" s="81"/>
+      <c r="N21" s="79"/>
+      <c r="O21" s="80"/>
+      <c r="P21" s="80"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="81"/>
     </row>
     <row r="22" spans="2:18">
-      <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="44"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="44"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="43"/>
-      <c r="Q22" s="43"/>
-      <c r="R22" s="44"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="81"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="81"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="80"/>
+      <c r="R22" s="81"/>
     </row>
     <row r="23" spans="2:18">
-      <c r="B23" s="45"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="47"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="47"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="47"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="84"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="83"/>
+      <c r="J23" s="83"/>
+      <c r="K23" s="83"/>
+      <c r="L23" s="84"/>
+      <c r="N23" s="82"/>
+      <c r="O23" s="83"/>
+      <c r="P23" s="83"/>
+      <c r="Q23" s="83"/>
+      <c r="R23" s="84"/>
     </row>
     <row r="26" spans="2:18" ht="18.3">
       <c r="B26" s="6" t="s">
@@ -3858,341 +4066,341 @@
     </row>
     <row r="37" spans="2:18" ht="14.7" thickBot="1"/>
     <row r="38" spans="2:18">
-      <c r="B38" s="58" t="s">
+      <c r="B38" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="60"/>
-      <c r="H38" s="76" t="s">
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="39"/>
+      <c r="H38" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="I38" s="77"/>
-      <c r="J38" s="77"/>
-      <c r="K38" s="77"/>
-      <c r="L38" s="78"/>
-      <c r="N38" s="70" t="s">
+      <c r="I38" s="86"/>
+      <c r="J38" s="86"/>
+      <c r="K38" s="86"/>
+      <c r="L38" s="87"/>
+      <c r="N38" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="O38" s="71"/>
-      <c r="P38" s="71"/>
-      <c r="Q38" s="71"/>
-      <c r="R38" s="72"/>
+      <c r="O38" s="50"/>
+      <c r="P38" s="50"/>
+      <c r="Q38" s="50"/>
+      <c r="R38" s="51"/>
     </row>
     <row r="39" spans="2:18" ht="14.7" thickBot="1">
-      <c r="B39" s="61"/>
-      <c r="C39" s="62"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="62"/>
-      <c r="F39" s="63"/>
-      <c r="H39" s="79"/>
-      <c r="I39" s="80"/>
-      <c r="J39" s="80"/>
-      <c r="K39" s="80"/>
-      <c r="L39" s="81"/>
-      <c r="N39" s="73"/>
-      <c r="O39" s="74"/>
-      <c r="P39" s="74"/>
-      <c r="Q39" s="74"/>
-      <c r="R39" s="75"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="42"/>
+      <c r="H39" s="88"/>
+      <c r="I39" s="89"/>
+      <c r="J39" s="89"/>
+      <c r="K39" s="89"/>
+      <c r="L39" s="90"/>
+      <c r="N39" s="52"/>
+      <c r="O39" s="53"/>
+      <c r="P39" s="53"/>
+      <c r="Q39" s="53"/>
+      <c r="R39" s="54"/>
     </row>
     <row r="40" spans="2:18">
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="51"/>
-      <c r="H40" s="49" t="s">
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="57"/>
+      <c r="H40" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="I40" s="50"/>
-      <c r="J40" s="50"/>
-      <c r="K40" s="50"/>
-      <c r="L40" s="51"/>
-      <c r="N40" s="49" t="s">
+      <c r="I40" s="56"/>
+      <c r="J40" s="56"/>
+      <c r="K40" s="56"/>
+      <c r="L40" s="57"/>
+      <c r="N40" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="O40" s="50"/>
-      <c r="P40" s="50"/>
-      <c r="Q40" s="50"/>
-      <c r="R40" s="51"/>
+      <c r="O40" s="56"/>
+      <c r="P40" s="56"/>
+      <c r="Q40" s="56"/>
+      <c r="R40" s="57"/>
     </row>
     <row r="41" spans="2:18">
-      <c r="B41" s="52"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="54"/>
-      <c r="H41" s="52"/>
-      <c r="I41" s="53"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="53"/>
-      <c r="L41" s="54"/>
-      <c r="N41" s="52"/>
-      <c r="O41" s="53"/>
-      <c r="P41" s="53"/>
-      <c r="Q41" s="53"/>
-      <c r="R41" s="54"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
+      <c r="F41" s="60"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="59"/>
+      <c r="J41" s="59"/>
+      <c r="K41" s="59"/>
+      <c r="L41" s="60"/>
+      <c r="N41" s="58"/>
+      <c r="O41" s="59"/>
+      <c r="P41" s="59"/>
+      <c r="Q41" s="59"/>
+      <c r="R41" s="60"/>
     </row>
     <row r="42" spans="2:18">
-      <c r="B42" s="52"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="54"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="54"/>
-      <c r="N42" s="52"/>
-      <c r="O42" s="53"/>
-      <c r="P42" s="53"/>
-      <c r="Q42" s="53"/>
-      <c r="R42" s="54"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="60"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="60"/>
+      <c r="N42" s="58"/>
+      <c r="O42" s="59"/>
+      <c r="P42" s="59"/>
+      <c r="Q42" s="59"/>
+      <c r="R42" s="60"/>
     </row>
     <row r="43" spans="2:18">
-      <c r="B43" s="55"/>
-      <c r="C43" s="56"/>
-      <c r="D43" s="56"/>
-      <c r="E43" s="56"/>
-      <c r="F43" s="57"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="56"/>
-      <c r="J43" s="56"/>
-      <c r="K43" s="56"/>
-      <c r="L43" s="57"/>
-      <c r="N43" s="55"/>
-      <c r="O43" s="56"/>
-      <c r="P43" s="56"/>
-      <c r="Q43" s="56"/>
-      <c r="R43" s="57"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="63"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="62"/>
+      <c r="L43" s="63"/>
+      <c r="N43" s="61"/>
+      <c r="O43" s="62"/>
+      <c r="P43" s="62"/>
+      <c r="Q43" s="62"/>
+      <c r="R43" s="63"/>
     </row>
     <row r="45" spans="2:18" ht="14.7" thickBot="1"/>
     <row r="46" spans="2:18" ht="16" customHeight="1">
-      <c r="B46" s="58" t="s">
+      <c r="B46" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="60"/>
-      <c r="H46" s="64" t="s">
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="39"/>
+      <c r="H46" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="I46" s="65"/>
-      <c r="J46" s="65"/>
-      <c r="K46" s="65"/>
-      <c r="L46" s="66"/>
-      <c r="N46" s="70" t="s">
+      <c r="I46" s="92"/>
+      <c r="J46" s="92"/>
+      <c r="K46" s="92"/>
+      <c r="L46" s="93"/>
+      <c r="N46" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="O46" s="71"/>
-      <c r="P46" s="71"/>
-      <c r="Q46" s="71"/>
-      <c r="R46" s="72"/>
+      <c r="O46" s="50"/>
+      <c r="P46" s="50"/>
+      <c r="Q46" s="50"/>
+      <c r="R46" s="51"/>
     </row>
     <row r="47" spans="2:18" ht="16" customHeight="1" thickBot="1">
-      <c r="B47" s="61"/>
-      <c r="C47" s="62"/>
-      <c r="D47" s="62"/>
-      <c r="E47" s="62"/>
-      <c r="F47" s="63"/>
-      <c r="H47" s="67"/>
-      <c r="I47" s="68"/>
-      <c r="J47" s="68"/>
-      <c r="K47" s="68"/>
-      <c r="L47" s="69"/>
-      <c r="N47" s="73"/>
-      <c r="O47" s="74"/>
-      <c r="P47" s="74"/>
-      <c r="Q47" s="74"/>
-      <c r="R47" s="75"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="42"/>
+      <c r="H47" s="94"/>
+      <c r="I47" s="95"/>
+      <c r="J47" s="95"/>
+      <c r="K47" s="95"/>
+      <c r="L47" s="96"/>
+      <c r="N47" s="52"/>
+      <c r="O47" s="53"/>
+      <c r="P47" s="53"/>
+      <c r="Q47" s="53"/>
+      <c r="R47" s="54"/>
     </row>
     <row r="48" spans="2:18">
-      <c r="B48" s="39" t="s">
+      <c r="B48" s="76" t="s">
         <v>123</v>
       </c>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="41"/>
-      <c r="H48" s="48" t="s">
+      <c r="C48" s="77"/>
+      <c r="D48" s="77"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="78"/>
+      <c r="H48" s="100" t="s">
         <v>124</v>
       </c>
-      <c r="I48" s="40"/>
-      <c r="J48" s="40"/>
-      <c r="K48" s="40"/>
-      <c r="L48" s="41"/>
-      <c r="N48" s="39" t="s">
+      <c r="I48" s="77"/>
+      <c r="J48" s="77"/>
+      <c r="K48" s="77"/>
+      <c r="L48" s="78"/>
+      <c r="N48" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="O48" s="40"/>
-      <c r="P48" s="40"/>
-      <c r="Q48" s="40"/>
-      <c r="R48" s="41"/>
+      <c r="O48" s="77"/>
+      <c r="P48" s="77"/>
+      <c r="Q48" s="77"/>
+      <c r="R48" s="78"/>
     </row>
     <row r="49" spans="2:18">
-      <c r="B49" s="42"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="44"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="44"/>
-      <c r="N49" s="42"/>
-      <c r="O49" s="43"/>
-      <c r="P49" s="43"/>
-      <c r="Q49" s="43"/>
-      <c r="R49" s="44"/>
+      <c r="B49" s="79"/>
+      <c r="C49" s="80"/>
+      <c r="D49" s="80"/>
+      <c r="E49" s="80"/>
+      <c r="F49" s="81"/>
+      <c r="H49" s="79"/>
+      <c r="I49" s="80"/>
+      <c r="J49" s="80"/>
+      <c r="K49" s="80"/>
+      <c r="L49" s="81"/>
+      <c r="N49" s="79"/>
+      <c r="O49" s="80"/>
+      <c r="P49" s="80"/>
+      <c r="Q49" s="80"/>
+      <c r="R49" s="81"/>
     </row>
     <row r="50" spans="2:18">
-      <c r="B50" s="42"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="44"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="44"/>
-      <c r="N50" s="42"/>
-      <c r="O50" s="43"/>
-      <c r="P50" s="43"/>
-      <c r="Q50" s="43"/>
-      <c r="R50" s="44"/>
+      <c r="B50" s="79"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="80"/>
+      <c r="E50" s="80"/>
+      <c r="F50" s="81"/>
+      <c r="H50" s="79"/>
+      <c r="I50" s="80"/>
+      <c r="J50" s="80"/>
+      <c r="K50" s="80"/>
+      <c r="L50" s="81"/>
+      <c r="N50" s="79"/>
+      <c r="O50" s="80"/>
+      <c r="P50" s="80"/>
+      <c r="Q50" s="80"/>
+      <c r="R50" s="81"/>
     </row>
     <row r="51" spans="2:18">
-      <c r="B51" s="42"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="44"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="43"/>
-      <c r="L51" s="44"/>
-      <c r="N51" s="42"/>
-      <c r="O51" s="43"/>
-      <c r="P51" s="43"/>
-      <c r="Q51" s="43"/>
-      <c r="R51" s="44"/>
+      <c r="B51" s="79"/>
+      <c r="C51" s="80"/>
+      <c r="D51" s="80"/>
+      <c r="E51" s="80"/>
+      <c r="F51" s="81"/>
+      <c r="H51" s="79"/>
+      <c r="I51" s="80"/>
+      <c r="J51" s="80"/>
+      <c r="K51" s="80"/>
+      <c r="L51" s="81"/>
+      <c r="N51" s="79"/>
+      <c r="O51" s="80"/>
+      <c r="P51" s="80"/>
+      <c r="Q51" s="80"/>
+      <c r="R51" s="81"/>
     </row>
     <row r="52" spans="2:18">
-      <c r="B52" s="45"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="47"/>
-      <c r="H52" s="45"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="46"/>
-      <c r="K52" s="46"/>
-      <c r="L52" s="47"/>
-      <c r="N52" s="45"/>
-      <c r="O52" s="46"/>
-      <c r="P52" s="46"/>
-      <c r="Q52" s="46"/>
-      <c r="R52" s="47"/>
+      <c r="B52" s="82"/>
+      <c r="C52" s="83"/>
+      <c r="D52" s="83"/>
+      <c r="E52" s="83"/>
+      <c r="F52" s="84"/>
+      <c r="H52" s="82"/>
+      <c r="I52" s="83"/>
+      <c r="J52" s="83"/>
+      <c r="K52" s="83"/>
+      <c r="L52" s="84"/>
+      <c r="N52" s="82"/>
+      <c r="O52" s="83"/>
+      <c r="P52" s="83"/>
+      <c r="Q52" s="83"/>
+      <c r="R52" s="84"/>
     </row>
     <row r="53" spans="2:18">
-      <c r="B53" s="39" t="s">
+      <c r="B53" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="41"/>
-      <c r="H53" s="39" t="s">
+      <c r="C53" s="77"/>
+      <c r="D53" s="77"/>
+      <c r="E53" s="77"/>
+      <c r="F53" s="78"/>
+      <c r="H53" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="I53" s="40"/>
-      <c r="J53" s="40"/>
-      <c r="K53" s="40"/>
-      <c r="L53" s="41"/>
-      <c r="N53" s="39" t="s">
+      <c r="I53" s="77"/>
+      <c r="J53" s="77"/>
+      <c r="K53" s="77"/>
+      <c r="L53" s="78"/>
+      <c r="N53" s="76" t="s">
         <v>128</v>
       </c>
-      <c r="O53" s="40"/>
-      <c r="P53" s="40"/>
-      <c r="Q53" s="40"/>
-      <c r="R53" s="41"/>
+      <c r="O53" s="77"/>
+      <c r="P53" s="77"/>
+      <c r="Q53" s="77"/>
+      <c r="R53" s="78"/>
     </row>
     <row r="54" spans="2:18">
-      <c r="B54" s="42"/>
-      <c r="C54" s="43"/>
-      <c r="D54" s="43"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="44"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="43"/>
-      <c r="J54" s="43"/>
-      <c r="K54" s="43"/>
-      <c r="L54" s="44"/>
-      <c r="N54" s="42"/>
-      <c r="O54" s="43"/>
-      <c r="P54" s="43"/>
-      <c r="Q54" s="43"/>
-      <c r="R54" s="44"/>
+      <c r="B54" s="79"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="80"/>
+      <c r="F54" s="81"/>
+      <c r="H54" s="79"/>
+      <c r="I54" s="80"/>
+      <c r="J54" s="80"/>
+      <c r="K54" s="80"/>
+      <c r="L54" s="81"/>
+      <c r="N54" s="79"/>
+      <c r="O54" s="80"/>
+      <c r="P54" s="80"/>
+      <c r="Q54" s="80"/>
+      <c r="R54" s="81"/>
     </row>
     <row r="55" spans="2:18">
-      <c r="B55" s="42"/>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="44"/>
-      <c r="H55" s="42"/>
-      <c r="I55" s="43"/>
-      <c r="J55" s="43"/>
-      <c r="K55" s="43"/>
-      <c r="L55" s="44"/>
-      <c r="N55" s="42"/>
-      <c r="O55" s="43"/>
-      <c r="P55" s="43"/>
-      <c r="Q55" s="43"/>
-      <c r="R55" s="44"/>
+      <c r="B55" s="79"/>
+      <c r="C55" s="80"/>
+      <c r="D55" s="80"/>
+      <c r="E55" s="80"/>
+      <c r="F55" s="81"/>
+      <c r="H55" s="79"/>
+      <c r="I55" s="80"/>
+      <c r="J55" s="80"/>
+      <c r="K55" s="80"/>
+      <c r="L55" s="81"/>
+      <c r="N55" s="79"/>
+      <c r="O55" s="80"/>
+      <c r="P55" s="80"/>
+      <c r="Q55" s="80"/>
+      <c r="R55" s="81"/>
     </row>
     <row r="56" spans="2:18">
-      <c r="B56" s="42"/>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="44"/>
-      <c r="H56" s="42"/>
-      <c r="I56" s="43"/>
-      <c r="J56" s="43"/>
-      <c r="K56" s="43"/>
-      <c r="L56" s="44"/>
-      <c r="N56" s="42"/>
-      <c r="O56" s="43"/>
-      <c r="P56" s="43"/>
-      <c r="Q56" s="43"/>
-      <c r="R56" s="44"/>
+      <c r="B56" s="79"/>
+      <c r="C56" s="80"/>
+      <c r="D56" s="80"/>
+      <c r="E56" s="80"/>
+      <c r="F56" s="81"/>
+      <c r="H56" s="79"/>
+      <c r="I56" s="80"/>
+      <c r="J56" s="80"/>
+      <c r="K56" s="80"/>
+      <c r="L56" s="81"/>
+      <c r="N56" s="79"/>
+      <c r="O56" s="80"/>
+      <c r="P56" s="80"/>
+      <c r="Q56" s="80"/>
+      <c r="R56" s="81"/>
     </row>
     <row r="57" spans="2:18">
-      <c r="B57" s="45"/>
-      <c r="C57" s="46"/>
-      <c r="D57" s="46"/>
-      <c r="E57" s="46"/>
-      <c r="F57" s="47"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="46"/>
-      <c r="J57" s="46"/>
-      <c r="K57" s="46"/>
-      <c r="L57" s="47"/>
-      <c r="N57" s="45"/>
-      <c r="O57" s="46"/>
-      <c r="P57" s="46"/>
-      <c r="Q57" s="46"/>
-      <c r="R57" s="47"/>
+      <c r="B57" s="82"/>
+      <c r="C57" s="83"/>
+      <c r="D57" s="83"/>
+      <c r="E57" s="83"/>
+      <c r="F57" s="84"/>
+      <c r="H57" s="82"/>
+      <c r="I57" s="83"/>
+      <c r="J57" s="83"/>
+      <c r="K57" s="83"/>
+      <c r="L57" s="84"/>
+      <c r="N57" s="82"/>
+      <c r="O57" s="83"/>
+      <c r="P57" s="83"/>
+      <c r="Q57" s="83"/>
+      <c r="R57" s="84"/>
     </row>
     <row r="60" spans="2:18" ht="18.3">
       <c r="B60" s="6" t="s">
@@ -4365,13 +4573,13 @@
       <c r="R67" s="27"/>
     </row>
     <row r="70" spans="2:18" ht="15.6">
-      <c r="N70" s="36" t="s">
+      <c r="N70" s="97" t="s">
         <v>143</v>
       </c>
-      <c r="O70" s="37"/>
-      <c r="P70" s="37"/>
-      <c r="Q70" s="37"/>
-      <c r="R70" s="38"/>
+      <c r="O70" s="98"/>
+      <c r="P70" s="98"/>
+      <c r="Q70" s="98"/>
+      <c r="R70" s="99"/>
     </row>
     <row r="71" spans="2:18" ht="32.1" customHeight="1">
       <c r="N71" s="28"/>
@@ -4446,30 +4654,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B4:F5"/>
-    <mergeCell ref="H4:L5"/>
-    <mergeCell ref="N4:R5"/>
-    <mergeCell ref="B6:F9"/>
-    <mergeCell ref="H6:L9"/>
-    <mergeCell ref="N6:R9"/>
-    <mergeCell ref="B12:F13"/>
-    <mergeCell ref="H12:L13"/>
-    <mergeCell ref="N12:R13"/>
-    <mergeCell ref="B14:F18"/>
-    <mergeCell ref="H14:L18"/>
-    <mergeCell ref="N14:R18"/>
-    <mergeCell ref="B19:F23"/>
-    <mergeCell ref="H19:L23"/>
-    <mergeCell ref="N19:R23"/>
-    <mergeCell ref="B38:F39"/>
-    <mergeCell ref="H38:L39"/>
-    <mergeCell ref="N38:R39"/>
-    <mergeCell ref="B40:F43"/>
-    <mergeCell ref="H40:L43"/>
-    <mergeCell ref="N40:R43"/>
-    <mergeCell ref="B46:F47"/>
-    <mergeCell ref="H46:L47"/>
-    <mergeCell ref="N46:R47"/>
     <mergeCell ref="N70:R70"/>
     <mergeCell ref="B48:F52"/>
     <mergeCell ref="H48:L52"/>
@@ -4477,6 +4661,30 @@
     <mergeCell ref="B53:F57"/>
     <mergeCell ref="H53:L57"/>
     <mergeCell ref="N53:R57"/>
+    <mergeCell ref="B40:F43"/>
+    <mergeCell ref="H40:L43"/>
+    <mergeCell ref="N40:R43"/>
+    <mergeCell ref="B46:F47"/>
+    <mergeCell ref="H46:L47"/>
+    <mergeCell ref="N46:R47"/>
+    <mergeCell ref="B19:F23"/>
+    <mergeCell ref="H19:L23"/>
+    <mergeCell ref="N19:R23"/>
+    <mergeCell ref="B38:F39"/>
+    <mergeCell ref="H38:L39"/>
+    <mergeCell ref="N38:R39"/>
+    <mergeCell ref="B12:F13"/>
+    <mergeCell ref="H12:L13"/>
+    <mergeCell ref="N12:R13"/>
+    <mergeCell ref="B14:F18"/>
+    <mergeCell ref="H14:L18"/>
+    <mergeCell ref="N14:R18"/>
+    <mergeCell ref="B4:F5"/>
+    <mergeCell ref="H4:L5"/>
+    <mergeCell ref="N4:R5"/>
+    <mergeCell ref="B6:F9"/>
+    <mergeCell ref="H6:L9"/>
+    <mergeCell ref="N6:R9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
aggiornamento quote as of EoMarch
</commit_message>
<xml_diff>
--- a/input/assets.xlsx
+++ b/input/assets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935cc860ba0efd68/GitHub/myportfolio/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:1_{B10D7187-5546-4483-8DEF-63838578FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4330DA66-9903-445E-84CC-CE3DE94180C9}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{B10D7187-5546-4483-8DEF-63838578FBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB0DF4A2-6088-45EE-B595-E79FDB27BE71}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="6" r:id="rId1"/>
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="234">
   <si>
     <t>Link</t>
   </si>
@@ -1291,6 +1291,15 @@
   </si>
   <si>
     <t>0.79</t>
+  </si>
+  <si>
+    <t>iShares Edge MSCI World Quality Factor UCITS ETF (Acc) | IWQU | IE00BP3QZ601</t>
+  </si>
+  <si>
+    <t>World Quality</t>
+  </si>
+  <si>
+    <t>come tutti gli etf azionari si hedgiano da soli, le aziende internaizonali adattano i prezzi in base al fx rate, quindi i bilanci si adattano accordingly etc.</t>
   </si>
 </sst>
 </file>
@@ -1720,11 +1729,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="103">
@@ -1784,122 +1792,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1928,60 +1829,166 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8"/>
-    <cellStyle name="Hyperlink" xfId="4" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 2" xfId="1" xr:uid="{72EA356F-0A49-47BB-9DAA-0B0102CDB9D4}"/>
     <cellStyle name="Valuta 2" xfId="2" xr:uid="{B87CA5A7-8DFB-4A60-8670-448CAC58448C}"/>
   </cellStyles>
@@ -2261,26 +2268,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B015881-81C4-40D2-9396-65046E56EE7C}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.15625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.41796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="255.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.15625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.15625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.83984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="255.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2382,7 +2389,7 @@
         <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1">
         <v>2.5000000000000001E-3</v>
@@ -2399,19 +2406,19 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="35" t="s">
-        <v>31</v>
+        <v>231</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>232</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>165</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2423,27 +2430,30 @@
         <v>19</v>
       </c>
       <c r="I4" s="1">
-        <v>2E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="J4" t="s">
         <v>30</v>
       </c>
+      <c r="L4" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="35" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -2455,27 +2465,27 @@
         <v>19</v>
       </c>
       <c r="I5" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15">
-      <c r="A6" s="102" t="s">
-        <v>41</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="35" t="s">
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -2487,24 +2497,27 @@
         <v>19</v>
       </c>
       <c r="I6" s="1">
-        <v>2.5000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="35" t="s">
-        <v>46</v>
+      <c r="A7" s="38" t="s">
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
         <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -2513,30 +2526,27 @@
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I7" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J7" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="35" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
@@ -2548,39 +2558,39 @@
         <v>29</v>
       </c>
       <c r="I8" s="1">
-        <v>3.5000000000000001E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="35" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>61</v>
+        <v>29</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="J9" t="s">
         <v>20</v>
@@ -2588,19 +2598,19 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="35" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
         <v>28</v>
@@ -2611,34 +2621,28 @@
       <c r="H10" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="1">
-        <v>1.5E-3</v>
+      <c r="I10" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="J10" t="s">
         <v>20</v>
       </c>
-      <c r="K10" t="s">
-        <v>67</v>
-      </c>
-      <c r="L10" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="35" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F11" t="s">
         <v>28</v>
@@ -2647,30 +2651,36 @@
         <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="I11" s="1">
-        <v>8.9999999999999998E-4</v>
+        <v>1.5E-3</v>
       </c>
       <c r="J11" t="s">
         <v>20</v>
       </c>
+      <c r="K11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="35" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s">
         <v>28</v>
@@ -2682,103 +2692,136 @@
         <v>29</v>
       </c>
       <c r="I12" s="1">
-        <v>1E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="J12" t="s">
-        <v>79</v>
-      </c>
-      <c r="K12" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="35" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s">
         <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="I13" s="1">
-        <v>6.9999999999999999E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J13" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="K13" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="35" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
         <v>18</v>
       </c>
       <c r="H14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="1">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="J14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I15" s="1">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J15" t="s">
         <v>30</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K15" t="s">
         <v>92</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L15" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B3VTN290" xr:uid="{6AB80B8F-0CAF-4297-B9BB-D72ED9AFBF01}"/>
-    <hyperlink ref="A13" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{69029A56-B54E-49FD-A0F5-77171229A26E}"/>
-    <hyperlink ref="A14" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B579F325" xr:uid="{42CB0A67-6EA5-4F8A-A191-29BAAE4A4956}"/>
-    <hyperlink ref="A4" r:id="rId4" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BD1F4L37" xr:uid="{DF84D7C7-B8F6-477A-8C9A-D4997B54C865}"/>
-    <hyperlink ref="A5" r:id="rId5" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B8FHGS14" xr:uid="{47A684AB-EAC0-4609-B6F5-2C135D16A87D}"/>
-    <hyperlink ref="A12" r:id="rId6" display="https://finance.yahoo.com/quote/LEONIA.MI/" xr:uid="{C03B49D3-5D8D-4719-818C-85A9CCE78BAE}"/>
-    <hyperlink ref="A11" r:id="rId7" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B0M62X26" xr:uid="{80E603FC-0B0D-4EAD-9D73-152F6C249FED}"/>
+    <hyperlink ref="A11" r:id="rId1" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B3VTN290" xr:uid="{6AB80B8F-0CAF-4297-B9BB-D72ED9AFBF01}"/>
+    <hyperlink ref="A14" r:id="rId2" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BGR7L912" xr:uid="{69029A56-B54E-49FD-A0F5-77171229A26E}"/>
+    <hyperlink ref="A15" r:id="rId3" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B579F325" xr:uid="{42CB0A67-6EA5-4F8A-A191-29BAAE4A4956}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BD1F4L37" xr:uid="{DF84D7C7-B8F6-477A-8C9A-D4997B54C865}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B8FHGS14" xr:uid="{47A684AB-EAC0-4609-B6F5-2C135D16A87D}"/>
+    <hyperlink ref="A13" r:id="rId6" display="https://finance.yahoo.com/quote/LEONIA.MI/" xr:uid="{C03B49D3-5D8D-4719-818C-85A9CCE78BAE}"/>
+    <hyperlink ref="A12" r:id="rId7" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B0M62X26" xr:uid="{80E603FC-0B0D-4EAD-9D73-152F6C249FED}"/>
     <hyperlink ref="A2" r:id="rId8" display="https://www.justetf.com/it/etf-profile.html?isin=IE00B4L5Y983" xr:uid="{07C799E5-4B70-419F-8A83-D91DFAD88307}"/>
     <hyperlink ref="A3" r:id="rId9" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BP3QZ825" xr:uid="{ED793FF2-3042-4018-9FA6-08360F193E0B}"/>
-    <hyperlink ref="A7" r:id="rId10" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BM67HN09" xr:uid="{2EEFD69B-BBC2-44B7-BDD8-699CB046D272}"/>
-    <hyperlink ref="A8" r:id="rId11" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BF4RFH31" xr:uid="{04A5FBD1-1EA4-45D6-A88A-DC1C0D39B403}"/>
-    <hyperlink ref="A9" r:id="rId12" display="https://www.justetf.com/it/etf-profile.html?isin=IE0032523478" xr:uid="{408B8EA9-ABA3-409D-8344-122D3BE0F3B9}"/>
-    <hyperlink ref="A6" r:id="rId13" xr:uid="{62F5217A-B11D-43D5-9707-F13957F40612}"/>
+    <hyperlink ref="A8" r:id="rId10" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BM67HN09" xr:uid="{2EEFD69B-BBC2-44B7-BDD8-699CB046D272}"/>
+    <hyperlink ref="A9" r:id="rId11" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BF4RFH31" xr:uid="{04A5FBD1-1EA4-45D6-A88A-DC1C0D39B403}"/>
+    <hyperlink ref="A10" r:id="rId12" display="https://www.justetf.com/it/etf-profile.html?isin=IE0032523478" xr:uid="{408B8EA9-ABA3-409D-8344-122D3BE0F3B9}"/>
+    <hyperlink ref="A7" r:id="rId13" xr:uid="{62F5217A-B11D-43D5-9707-F13957F40612}"/>
+    <hyperlink ref="A4" r:id="rId14" display="https://www.justetf.com/it/etf-profile.html?isin=IE00BP3QZ601" xr:uid="{1C774625-8FE5-4E4F-8DCA-3CDE0AD177A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2792,17 +2835,17 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="55.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.41796875" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3209,10 +3252,10 @@
       <selection activeCell="A13" sqref="A13:J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="3" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.68359375" customWidth="1"/>
+    <col min="3" max="3" width="52.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3689,19 +3732,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939D994C-0E7B-435F-BB4C-7162BD8072E3}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A14">overview!E1:E14</f>
+        <f t="array" ref="A1:A15">overview!E1:E15</f>
         <v>Ticker</v>
       </c>
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:B14">overview!B1:B14</f>
+        <f t="array" ref="B1:B15">overview!B1:B15</f>
         <v>Index</v>
       </c>
     </row>
@@ -3723,89 +3766,97 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="str">
-        <v>QDVB.DE</v>
+        <v>IWQU.L</v>
       </c>
       <c r="B4" t="str">
-        <v>US Quality</v>
+        <v>World Quality</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="str">
-        <v>MVOL.L</v>
+        <v>QDVB.DE</v>
       </c>
       <c r="B5" t="str">
-        <v>World Low Volatility</v>
+        <v>US Quality</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="str">
-        <v>XDWH.MI</v>
+        <v>MVOL.L</v>
       </c>
       <c r="B6" t="str">
-        <v>World Health Care</v>
+        <v>World Low Volatility</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="str">
-        <v>XDWS.L</v>
+        <v>XDWH.MI</v>
       </c>
       <c r="B7" t="str">
-        <v>Consumer Staples Global</v>
+        <v>World Health Care</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="str">
-        <v>WSML.L</v>
+        <v>XDWS.L</v>
       </c>
       <c r="B8" t="str">
-        <v>Small Cap Global</v>
+        <v>Consumer Staples Global</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="str">
-        <v>IBCX.AS</v>
+        <v>WSML.L</v>
       </c>
       <c r="B9" t="str">
-        <v>EU Corp Large Cap bonds</v>
+        <v>Small Cap Global</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="str">
-        <v>IBGM.AS</v>
+        <v>IBCX.AS</v>
       </c>
       <c r="B10" t="str">
-        <v>EU Gov bonds 7-10y</v>
+        <v>EU Corp Large Cap bonds</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="str">
-        <v>IBCI.AS</v>
+        <v>IBGM.AS</v>
       </c>
       <c r="B11" t="str">
-        <v>EU Inflation-Linked</v>
+        <v>EU Gov bonds 7-10y</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="str">
-        <v>LEONIA.MI</v>
+        <v>IBCI.AS</v>
       </c>
       <c r="B12" t="str">
-        <v>EU Overnight</v>
+        <v>EU Inflation-Linked</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="str">
-        <v>IBTU.L</v>
+        <v>LEONIA.MI</v>
       </c>
       <c r="B13" t="str">
-        <v>US Short Treasury</v>
+        <v>EU Overnight</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="str">
+        <v>IBTU.L</v>
+      </c>
+      <c r="B14" t="str">
+        <v>US Short Treasury</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="str">
         <v>SGLD.AS</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B15" t="str">
         <v>ETC GOLD</v>
       </c>
     </row>
@@ -3816,17 +3867,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA57C457-A80C-477F-8A3E-0F8DB96F6511}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A14">overview!C1:C14</f>
+        <f t="array" ref="A1:A15">overview!C1:C15</f>
         <v>Name</v>
       </c>
     </row>
@@ -3842,56 +3893,61 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="str">
-        <v>iShares Edge MSCI USA Quality Factor UCITS ETF</v>
+        <v>iShares Edge MSCI World Quality Factor UCITS ETF (Acc)</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="str">
-        <v>iShares Edge MSCI World Minimum Volatility UCITS ETF USD (Acc)</v>
+        <v>iShares Edge MSCI USA Quality Factor UCITS ETF</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="str">
-        <v>Xtrackers MSCI World Health Care UCITS ETF 1C</v>
+        <v>iShares Edge MSCI World Minimum Volatility UCITS ETF USD (Acc)</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="str">
-        <v>Xtrackers MSCI World Consumer Staples UCITS ETF (Acc)</v>
+        <v>Xtrackers MSCI World Health Care UCITS ETF 1C</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="str">
-        <v>iShares MSCI World Small Cap UCITS ETF</v>
+        <v>Xtrackers MSCI World Consumer Staples UCITS ETF (Acc)</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="str">
-        <v>iShares Euro Corporate Bond Large Cap UCITS ETF</v>
+        <v>iShares MSCI World Small Cap UCITS ETF</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="str">
-        <v>iShares € Govt Bond 7-10yr UCITS ETF EUR (Dist)</v>
+        <v>iShares Euro Corporate Bond Large Cap UCITS ETF</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="str">
-        <v>iShares € Inflation Linked Govt Bond UCITS ETF EUR (Acc)</v>
+        <v>iShares € Govt Bond 7-10yr UCITS ETF EUR (Dist)</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="str">
-        <v>Amundi EUR Overnight Return UCITS ETF Acc</v>
+        <v>iShares € Inflation Linked Govt Bond UCITS ETF EUR (Acc)</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="str">
-        <v>iShares USD Treasury Bond 0-1yr UCITS ETF (Dist)</v>
+        <v>Amundi EUR Overnight Return UCITS ETF Acc</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="str">
+        <v>iShares USD Treasury Bond 0-1yr UCITS ETF (Dist)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="str">
         <v>Invesco Physical Gold ETC</v>
       </c>
     </row>
@@ -3908,10 +3964,10 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="87.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="87.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -4139,130 +4195,130 @@
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.15">
+    <row r="1" spans="1:18" ht="25.2">
       <c r="A1" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="25.15">
+    <row r="2" spans="1:18" ht="25.2">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="14.65" thickBot="1"/>
-    <row r="4" spans="1:18" ht="15.95" customHeight="1">
-      <c r="B4" s="38" t="s">
+    <row r="3" spans="1:18" ht="14.7" thickBot="1"/>
+    <row r="4" spans="1:18" ht="16" customHeight="1">
+      <c r="B4" s="61" t="s">
         <v>177</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
-      <c r="H4" s="44" t="s">
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="63"/>
+      <c r="H4" s="97" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="46"/>
-      <c r="N4" s="50" t="s">
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="99"/>
+      <c r="N4" s="73" t="s">
         <v>179</v>
       </c>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="52"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="75"/>
     </row>
     <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="49"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="55"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="66"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="102"/>
+      <c r="N5" s="76"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
+      <c r="R5" s="78"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="58"/>
-      <c r="H6" s="56" t="s">
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="54"/>
+      <c r="H6" s="52" t="s">
         <v>181</v>
       </c>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="58"/>
-      <c r="N6" s="56" t="s">
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="54"/>
+      <c r="N6" s="52" t="s">
         <v>181</v>
       </c>
-      <c r="O6" s="57"/>
-      <c r="P6" s="57"/>
-      <c r="Q6" s="57"/>
-      <c r="R6" s="58"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="54"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="B7" s="59"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="61"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="61"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="60"/>
-      <c r="R7" s="61"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="57"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="57"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="B8" s="59"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="61"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="61"/>
-      <c r="N8" s="59"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="61"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="57"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="57"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="57"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="B9" s="62"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="64"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="64"/>
-      <c r="N9" s="62"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="64"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="60"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="60"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="59"/>
+      <c r="Q9" s="59"/>
+      <c r="R9" s="60"/>
     </row>
     <row r="10" spans="1:18">
       <c r="B10" s="37"/>
@@ -4281,230 +4337,230 @@
       <c r="Q10" s="37"/>
       <c r="R10" s="37"/>
     </row>
-    <row r="11" spans="1:18" ht="14.65" thickBot="1"/>
-    <row r="12" spans="1:18" ht="15.95" customHeight="1">
-      <c r="B12" s="38" t="s">
+    <row r="11" spans="1:18" ht="14.7" thickBot="1"/>
+    <row r="12" spans="1:18" ht="16" customHeight="1">
+      <c r="B12" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40"/>
-      <c r="H12" s="65" t="s">
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="63"/>
+      <c r="H12" s="85" t="s">
         <v>182</v>
       </c>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="67"/>
-      <c r="N12" s="71" t="s">
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="87"/>
+      <c r="N12" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="O12" s="72"/>
-      <c r="P12" s="72"/>
-      <c r="Q12" s="72"/>
-      <c r="R12" s="73"/>
-    </row>
-    <row r="13" spans="1:18" ht="15.95" customHeight="1">
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="70"/>
-      <c r="N13" s="74"/>
-      <c r="O13" s="75"/>
-      <c r="P13" s="75"/>
-      <c r="Q13" s="75"/>
-      <c r="R13" s="76"/>
-    </row>
-    <row r="14" spans="1:18" ht="15.95" customHeight="1">
-      <c r="B14" s="77" t="s">
+      <c r="O12" s="92"/>
+      <c r="P12" s="92"/>
+      <c r="Q12" s="92"/>
+      <c r="R12" s="93"/>
+    </row>
+    <row r="13" spans="1:18" ht="16" customHeight="1">
+      <c r="B13" s="64"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="90"/>
+      <c r="N13" s="94"/>
+      <c r="O13" s="95"/>
+      <c r="P13" s="95"/>
+      <c r="Q13" s="95"/>
+      <c r="R13" s="96"/>
+    </row>
+    <row r="14" spans="1:18" ht="16" customHeight="1">
+      <c r="B14" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="79"/>
-      <c r="H14" s="77" t="s">
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="44"/>
+      <c r="H14" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="79"/>
-      <c r="N14" s="77" t="s">
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="44"/>
+      <c r="N14" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="O14" s="78"/>
-      <c r="P14" s="78"/>
-      <c r="Q14" s="78"/>
-      <c r="R14" s="79"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="44"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="B15" s="80"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="82"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="81"/>
-      <c r="L15" s="82"/>
-      <c r="N15" s="80"/>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="82"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="47"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="47"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="46"/>
+      <c r="Q15" s="46"/>
+      <c r="R15" s="47"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="B16" s="80"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="82"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="82"/>
-      <c r="N16" s="80"/>
-      <c r="O16" s="81"/>
-      <c r="P16" s="81"/>
-      <c r="Q16" s="81"/>
-      <c r="R16" s="82"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="47"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="47"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="46"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="47"/>
     </row>
     <row r="17" spans="2:18">
-      <c r="B17" s="80"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="82"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="81"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="81"/>
-      <c r="L17" s="82"/>
-      <c r="N17" s="80"/>
-      <c r="O17" s="81"/>
-      <c r="P17" s="81"/>
-      <c r="Q17" s="81"/>
-      <c r="R17" s="82"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="47"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="47"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="47"/>
     </row>
     <row r="18" spans="2:18">
-      <c r="B18" s="83"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="85"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
-      <c r="K18" s="84"/>
-      <c r="L18" s="85"/>
-      <c r="N18" s="83"/>
-      <c r="O18" s="84"/>
-      <c r="P18" s="84"/>
-      <c r="Q18" s="84"/>
-      <c r="R18" s="85"/>
-    </row>
-    <row r="19" spans="2:18" ht="15.95" customHeight="1">
-      <c r="B19" s="77" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="50"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="50"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="50"/>
+    </row>
+    <row r="19" spans="2:18" ht="16" customHeight="1">
+      <c r="B19" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="79"/>
-      <c r="H19" s="77" t="s">
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="44"/>
+      <c r="H19" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="79"/>
-      <c r="N19" s="77" t="s">
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="44"/>
+      <c r="N19" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="O19" s="78"/>
-      <c r="P19" s="78"/>
-      <c r="Q19" s="78"/>
-      <c r="R19" s="79"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="44"/>
     </row>
     <row r="20" spans="2:18">
-      <c r="B20" s="80"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="82"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="82"/>
-      <c r="N20" s="80"/>
-      <c r="O20" s="81"/>
-      <c r="P20" s="81"/>
-      <c r="Q20" s="81"/>
-      <c r="R20" s="82"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="47"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="47"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="46"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="47"/>
     </row>
     <row r="21" spans="2:18">
-      <c r="B21" s="80"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="82"/>
-      <c r="H21" s="80"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="82"/>
-      <c r="N21" s="80"/>
-      <c r="O21" s="81"/>
-      <c r="P21" s="81"/>
-      <c r="Q21" s="81"/>
-      <c r="R21" s="82"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="47"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="47"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="47"/>
     </row>
     <row r="22" spans="2:18">
-      <c r="B22" s="80"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="82"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="82"/>
-      <c r="N22" s="80"/>
-      <c r="O22" s="81"/>
-      <c r="P22" s="81"/>
-      <c r="Q22" s="81"/>
-      <c r="R22" s="82"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="47"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="47"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="46"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="47"/>
     </row>
     <row r="23" spans="2:18">
-      <c r="B23" s="83"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="85"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="84"/>
-      <c r="L23" s="85"/>
-      <c r="N23" s="83"/>
-      <c r="O23" s="84"/>
-      <c r="P23" s="84"/>
-      <c r="Q23" s="84"/>
-      <c r="R23" s="85"/>
-    </row>
-    <row r="26" spans="2:18" ht="18.399999999999999">
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="50"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="50"/>
+    </row>
+    <row r="26" spans="2:18" ht="18.3">
       <c r="B26" s="5" t="s">
         <v>188</v>
       </c>
@@ -4666,345 +4722,345 @@
       <c r="Q33" s="12"/>
       <c r="R33" s="13"/>
     </row>
-    <row r="37" spans="2:18" ht="14.65" thickBot="1"/>
+    <row r="37" spans="2:18" ht="14.7" thickBot="1"/>
     <row r="38" spans="2:18">
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="40"/>
-      <c r="H38" s="86" t="s">
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="63"/>
+      <c r="H38" s="79" t="s">
         <v>198</v>
       </c>
-      <c r="I38" s="87"/>
-      <c r="J38" s="87"/>
-      <c r="K38" s="87"/>
-      <c r="L38" s="88"/>
-      <c r="N38" s="50" t="s">
+      <c r="I38" s="80"/>
+      <c r="J38" s="80"/>
+      <c r="K38" s="80"/>
+      <c r="L38" s="81"/>
+      <c r="N38" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="O38" s="51"/>
-      <c r="P38" s="51"/>
-      <c r="Q38" s="51"/>
-      <c r="R38" s="52"/>
-    </row>
-    <row r="39" spans="2:18" ht="14.65" thickBot="1">
-      <c r="B39" s="41"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="43"/>
-      <c r="H39" s="89"/>
-      <c r="I39" s="90"/>
-      <c r="J39" s="90"/>
-      <c r="K39" s="90"/>
-      <c r="L39" s="91"/>
-      <c r="N39" s="53"/>
-      <c r="O39" s="54"/>
-      <c r="P39" s="54"/>
-      <c r="Q39" s="54"/>
-      <c r="R39" s="55"/>
+      <c r="O38" s="74"/>
+      <c r="P38" s="74"/>
+      <c r="Q38" s="74"/>
+      <c r="R38" s="75"/>
+    </row>
+    <row r="39" spans="2:18" ht="14.7" thickBot="1">
+      <c r="B39" s="64"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="66"/>
+      <c r="H39" s="82"/>
+      <c r="I39" s="83"/>
+      <c r="J39" s="83"/>
+      <c r="K39" s="83"/>
+      <c r="L39" s="84"/>
+      <c r="N39" s="76"/>
+      <c r="O39" s="77"/>
+      <c r="P39" s="77"/>
+      <c r="Q39" s="77"/>
+      <c r="R39" s="78"/>
     </row>
     <row r="40" spans="2:18">
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="C40" s="57"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="58"/>
-      <c r="H40" s="56" t="s">
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="54"/>
+      <c r="H40" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="I40" s="57"/>
-      <c r="J40" s="57"/>
-      <c r="K40" s="57"/>
-      <c r="L40" s="58"/>
-      <c r="N40" s="56" t="s">
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="54"/>
+      <c r="N40" s="52" t="s">
         <v>202</v>
       </c>
-      <c r="O40" s="57"/>
-      <c r="P40" s="57"/>
-      <c r="Q40" s="57"/>
-      <c r="R40" s="58"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="53"/>
+      <c r="Q40" s="53"/>
+      <c r="R40" s="54"/>
     </row>
     <row r="41" spans="2:18">
-      <c r="B41" s="59"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="61"/>
-      <c r="H41" s="59"/>
-      <c r="I41" s="60"/>
-      <c r="J41" s="60"/>
-      <c r="K41" s="60"/>
-      <c r="L41" s="61"/>
-      <c r="N41" s="59"/>
-      <c r="O41" s="60"/>
-      <c r="P41" s="60"/>
-      <c r="Q41" s="60"/>
-      <c r="R41" s="61"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="57"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="56"/>
+      <c r="J41" s="56"/>
+      <c r="K41" s="56"/>
+      <c r="L41" s="57"/>
+      <c r="N41" s="55"/>
+      <c r="O41" s="56"/>
+      <c r="P41" s="56"/>
+      <c r="Q41" s="56"/>
+      <c r="R41" s="57"/>
     </row>
     <row r="42" spans="2:18">
-      <c r="B42" s="59"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="61"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="60"/>
-      <c r="J42" s="60"/>
-      <c r="K42" s="60"/>
-      <c r="L42" s="61"/>
-      <c r="N42" s="59"/>
-      <c r="O42" s="60"/>
-      <c r="P42" s="60"/>
-      <c r="Q42" s="60"/>
-      <c r="R42" s="61"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="57"/>
+      <c r="H42" s="55"/>
+      <c r="I42" s="56"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="56"/>
+      <c r="L42" s="57"/>
+      <c r="N42" s="55"/>
+      <c r="O42" s="56"/>
+      <c r="P42" s="56"/>
+      <c r="Q42" s="56"/>
+      <c r="R42" s="57"/>
     </row>
     <row r="43" spans="2:18">
-      <c r="B43" s="62"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="64"/>
-      <c r="H43" s="62"/>
-      <c r="I43" s="63"/>
-      <c r="J43" s="63"/>
-      <c r="K43" s="63"/>
-      <c r="L43" s="64"/>
-      <c r="N43" s="62"/>
-      <c r="O43" s="63"/>
-      <c r="P43" s="63"/>
-      <c r="Q43" s="63"/>
-      <c r="R43" s="64"/>
-    </row>
-    <row r="45" spans="2:18" ht="14.65" thickBot="1"/>
-    <row r="46" spans="2:18" ht="15.95" customHeight="1">
-      <c r="B46" s="38" t="s">
+      <c r="B43" s="58"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="60"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="59"/>
+      <c r="J43" s="59"/>
+      <c r="K43" s="59"/>
+      <c r="L43" s="60"/>
+      <c r="N43" s="58"/>
+      <c r="O43" s="59"/>
+      <c r="P43" s="59"/>
+      <c r="Q43" s="59"/>
+      <c r="R43" s="60"/>
+    </row>
+    <row r="45" spans="2:18" ht="14.7" thickBot="1"/>
+    <row r="46" spans="2:18" ht="16" customHeight="1">
+      <c r="B46" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="40"/>
-      <c r="H46" s="92" t="s">
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="62"/>
+      <c r="F46" s="63"/>
+      <c r="H46" s="67" t="s">
         <v>182</v>
       </c>
-      <c r="I46" s="93"/>
-      <c r="J46" s="93"/>
-      <c r="K46" s="93"/>
-      <c r="L46" s="94"/>
-      <c r="N46" s="50" t="s">
+      <c r="I46" s="68"/>
+      <c r="J46" s="68"/>
+      <c r="K46" s="68"/>
+      <c r="L46" s="69"/>
+      <c r="N46" s="73" t="s">
         <v>182</v>
       </c>
-      <c r="O46" s="51"/>
-      <c r="P46" s="51"/>
-      <c r="Q46" s="51"/>
-      <c r="R46" s="52"/>
-    </row>
-    <row r="47" spans="2:18" ht="15.95" customHeight="1" thickBot="1">
-      <c r="B47" s="41"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="43"/>
-      <c r="H47" s="95"/>
-      <c r="I47" s="96"/>
-      <c r="J47" s="96"/>
-      <c r="K47" s="96"/>
-      <c r="L47" s="97"/>
-      <c r="N47" s="53"/>
-      <c r="O47" s="54"/>
-      <c r="P47" s="54"/>
-      <c r="Q47" s="54"/>
-      <c r="R47" s="55"/>
+      <c r="O46" s="74"/>
+      <c r="P46" s="74"/>
+      <c r="Q46" s="74"/>
+      <c r="R46" s="75"/>
+    </row>
+    <row r="47" spans="2:18" ht="16" customHeight="1" thickBot="1">
+      <c r="B47" s="64"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="65"/>
+      <c r="F47" s="66"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="71"/>
+      <c r="J47" s="71"/>
+      <c r="K47" s="71"/>
+      <c r="L47" s="72"/>
+      <c r="N47" s="76"/>
+      <c r="O47" s="77"/>
+      <c r="P47" s="77"/>
+      <c r="Q47" s="77"/>
+      <c r="R47" s="78"/>
     </row>
     <row r="48" spans="2:18">
-      <c r="B48" s="77" t="s">
+      <c r="B48" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="C48" s="78"/>
-      <c r="D48" s="78"/>
-      <c r="E48" s="78"/>
-      <c r="F48" s="79"/>
-      <c r="H48" s="101" t="s">
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="44"/>
+      <c r="H48" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="I48" s="78"/>
-      <c r="J48" s="78"/>
-      <c r="K48" s="78"/>
-      <c r="L48" s="79"/>
-      <c r="N48" s="77" t="s">
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="44"/>
+      <c r="N48" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="O48" s="78"/>
-      <c r="P48" s="78"/>
-      <c r="Q48" s="78"/>
-      <c r="R48" s="79"/>
+      <c r="O48" s="43"/>
+      <c r="P48" s="43"/>
+      <c r="Q48" s="43"/>
+      <c r="R48" s="44"/>
     </row>
     <row r="49" spans="2:18">
-      <c r="B49" s="80"/>
-      <c r="C49" s="81"/>
-      <c r="D49" s="81"/>
-      <c r="E49" s="81"/>
-      <c r="F49" s="82"/>
-      <c r="H49" s="80"/>
-      <c r="I49" s="81"/>
-      <c r="J49" s="81"/>
-      <c r="K49" s="81"/>
-      <c r="L49" s="82"/>
-      <c r="N49" s="80"/>
-      <c r="O49" s="81"/>
-      <c r="P49" s="81"/>
-      <c r="Q49" s="81"/>
-      <c r="R49" s="82"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="47"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="46"/>
+      <c r="J49" s="46"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="47"/>
+      <c r="N49" s="45"/>
+      <c r="O49" s="46"/>
+      <c r="P49" s="46"/>
+      <c r="Q49" s="46"/>
+      <c r="R49" s="47"/>
     </row>
     <row r="50" spans="2:18">
-      <c r="B50" s="80"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="81"/>
-      <c r="E50" s="81"/>
-      <c r="F50" s="82"/>
-      <c r="H50" s="80"/>
-      <c r="I50" s="81"/>
-      <c r="J50" s="81"/>
-      <c r="K50" s="81"/>
-      <c r="L50" s="82"/>
-      <c r="N50" s="80"/>
-      <c r="O50" s="81"/>
-      <c r="P50" s="81"/>
-      <c r="Q50" s="81"/>
-      <c r="R50" s="82"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="47"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="47"/>
+      <c r="N50" s="45"/>
+      <c r="O50" s="46"/>
+      <c r="P50" s="46"/>
+      <c r="Q50" s="46"/>
+      <c r="R50" s="47"/>
     </row>
     <row r="51" spans="2:18">
-      <c r="B51" s="80"/>
-      <c r="C51" s="81"/>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81"/>
-      <c r="F51" s="82"/>
-      <c r="H51" s="80"/>
-      <c r="I51" s="81"/>
-      <c r="J51" s="81"/>
-      <c r="K51" s="81"/>
-      <c r="L51" s="82"/>
-      <c r="N51" s="80"/>
-      <c r="O51" s="81"/>
-      <c r="P51" s="81"/>
-      <c r="Q51" s="81"/>
-      <c r="R51" s="82"/>
+      <c r="B51" s="45"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="47"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="47"/>
+      <c r="N51" s="45"/>
+      <c r="O51" s="46"/>
+      <c r="P51" s="46"/>
+      <c r="Q51" s="46"/>
+      <c r="R51" s="47"/>
     </row>
     <row r="52" spans="2:18">
-      <c r="B52" s="83"/>
-      <c r="C52" s="84"/>
-      <c r="D52" s="84"/>
-      <c r="E52" s="84"/>
-      <c r="F52" s="85"/>
-      <c r="H52" s="83"/>
-      <c r="I52" s="84"/>
-      <c r="J52" s="84"/>
-      <c r="K52" s="84"/>
-      <c r="L52" s="85"/>
-      <c r="N52" s="83"/>
-      <c r="O52" s="84"/>
-      <c r="P52" s="84"/>
-      <c r="Q52" s="84"/>
-      <c r="R52" s="85"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="50"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="49"/>
+      <c r="J52" s="49"/>
+      <c r="K52" s="49"/>
+      <c r="L52" s="50"/>
+      <c r="N52" s="48"/>
+      <c r="O52" s="49"/>
+      <c r="P52" s="49"/>
+      <c r="Q52" s="49"/>
+      <c r="R52" s="50"/>
     </row>
     <row r="53" spans="2:18">
-      <c r="B53" s="77" t="s">
+      <c r="B53" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="C53" s="78"/>
-      <c r="D53" s="78"/>
-      <c r="E53" s="78"/>
-      <c r="F53" s="79"/>
-      <c r="H53" s="77" t="s">
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="44"/>
+      <c r="H53" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="I53" s="78"/>
-      <c r="J53" s="78"/>
-      <c r="K53" s="78"/>
-      <c r="L53" s="79"/>
-      <c r="N53" s="77" t="s">
+      <c r="I53" s="43"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="44"/>
+      <c r="N53" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="O53" s="78"/>
-      <c r="P53" s="78"/>
-      <c r="Q53" s="78"/>
-      <c r="R53" s="79"/>
+      <c r="O53" s="43"/>
+      <c r="P53" s="43"/>
+      <c r="Q53" s="43"/>
+      <c r="R53" s="44"/>
     </row>
     <row r="54" spans="2:18">
-      <c r="B54" s="80"/>
-      <c r="C54" s="81"/>
-      <c r="D54" s="81"/>
-      <c r="E54" s="81"/>
-      <c r="F54" s="82"/>
-      <c r="H54" s="80"/>
-      <c r="I54" s="81"/>
-      <c r="J54" s="81"/>
-      <c r="K54" s="81"/>
-      <c r="L54" s="82"/>
-      <c r="N54" s="80"/>
-      <c r="O54" s="81"/>
-      <c r="P54" s="81"/>
-      <c r="Q54" s="81"/>
-      <c r="R54" s="82"/>
+      <c r="B54" s="45"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="47"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="46"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="47"/>
+      <c r="N54" s="45"/>
+      <c r="O54" s="46"/>
+      <c r="P54" s="46"/>
+      <c r="Q54" s="46"/>
+      <c r="R54" s="47"/>
     </row>
     <row r="55" spans="2:18">
-      <c r="B55" s="80"/>
-      <c r="C55" s="81"/>
-      <c r="D55" s="81"/>
-      <c r="E55" s="81"/>
-      <c r="F55" s="82"/>
-      <c r="H55" s="80"/>
-      <c r="I55" s="81"/>
-      <c r="J55" s="81"/>
-      <c r="K55" s="81"/>
-      <c r="L55" s="82"/>
-      <c r="N55" s="80"/>
-      <c r="O55" s="81"/>
-      <c r="P55" s="81"/>
-      <c r="Q55" s="81"/>
-      <c r="R55" s="82"/>
+      <c r="B55" s="45"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="46"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="47"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="46"/>
+      <c r="J55" s="46"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="47"/>
+      <c r="N55" s="45"/>
+      <c r="O55" s="46"/>
+      <c r="P55" s="46"/>
+      <c r="Q55" s="46"/>
+      <c r="R55" s="47"/>
     </row>
     <row r="56" spans="2:18">
-      <c r="B56" s="80"/>
-      <c r="C56" s="81"/>
-      <c r="D56" s="81"/>
-      <c r="E56" s="81"/>
-      <c r="F56" s="82"/>
-      <c r="H56" s="80"/>
-      <c r="I56" s="81"/>
-      <c r="J56" s="81"/>
-      <c r="K56" s="81"/>
-      <c r="L56" s="82"/>
-      <c r="N56" s="80"/>
-      <c r="O56" s="81"/>
-      <c r="P56" s="81"/>
-      <c r="Q56" s="81"/>
-      <c r="R56" s="82"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="47"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="46"/>
+      <c r="J56" s="46"/>
+      <c r="K56" s="46"/>
+      <c r="L56" s="47"/>
+      <c r="N56" s="45"/>
+      <c r="O56" s="46"/>
+      <c r="P56" s="46"/>
+      <c r="Q56" s="46"/>
+      <c r="R56" s="47"/>
     </row>
     <row r="57" spans="2:18">
-      <c r="B57" s="83"/>
-      <c r="C57" s="84"/>
-      <c r="D57" s="84"/>
-      <c r="E57" s="84"/>
-      <c r="F57" s="85"/>
-      <c r="H57" s="83"/>
-      <c r="I57" s="84"/>
-      <c r="J57" s="84"/>
-      <c r="K57" s="84"/>
-      <c r="L57" s="85"/>
-      <c r="N57" s="83"/>
-      <c r="O57" s="84"/>
-      <c r="P57" s="84"/>
-      <c r="Q57" s="84"/>
-      <c r="R57" s="85"/>
-    </row>
-    <row r="60" spans="2:18" ht="18.399999999999999">
+      <c r="B57" s="48"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="49"/>
+      <c r="E57" s="49"/>
+      <c r="F57" s="50"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="49"/>
+      <c r="J57" s="49"/>
+      <c r="K57" s="49"/>
+      <c r="L57" s="50"/>
+      <c r="N57" s="48"/>
+      <c r="O57" s="49"/>
+      <c r="P57" s="49"/>
+      <c r="Q57" s="49"/>
+      <c r="R57" s="50"/>
+    </row>
+    <row r="60" spans="2:18" ht="18.3">
       <c r="B60" s="5" t="s">
         <v>188</v>
       </c>
@@ -5175,13 +5231,13 @@
       <c r="R67" s="26"/>
     </row>
     <row r="70" spans="2:18" ht="15.6">
-      <c r="N70" s="98" t="s">
+      <c r="N70" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="O70" s="99"/>
-      <c r="P70" s="99"/>
-      <c r="Q70" s="99"/>
-      <c r="R70" s="100"/>
+      <c r="O70" s="40"/>
+      <c r="P70" s="40"/>
+      <c r="Q70" s="40"/>
+      <c r="R70" s="41"/>
     </row>
     <row r="71" spans="2:18" ht="32.1" customHeight="1">
       <c r="N71" s="27"/>
@@ -5256,6 +5312,30 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B4:F5"/>
+    <mergeCell ref="H4:L5"/>
+    <mergeCell ref="N4:R5"/>
+    <mergeCell ref="B6:F9"/>
+    <mergeCell ref="H6:L9"/>
+    <mergeCell ref="N6:R9"/>
+    <mergeCell ref="B12:F13"/>
+    <mergeCell ref="H12:L13"/>
+    <mergeCell ref="N12:R13"/>
+    <mergeCell ref="B14:F18"/>
+    <mergeCell ref="H14:L18"/>
+    <mergeCell ref="N14:R18"/>
+    <mergeCell ref="B19:F23"/>
+    <mergeCell ref="H19:L23"/>
+    <mergeCell ref="N19:R23"/>
+    <mergeCell ref="B38:F39"/>
+    <mergeCell ref="H38:L39"/>
+    <mergeCell ref="N38:R39"/>
+    <mergeCell ref="B40:F43"/>
+    <mergeCell ref="H40:L43"/>
+    <mergeCell ref="N40:R43"/>
+    <mergeCell ref="B46:F47"/>
+    <mergeCell ref="H46:L47"/>
+    <mergeCell ref="N46:R47"/>
     <mergeCell ref="N70:R70"/>
     <mergeCell ref="B48:F52"/>
     <mergeCell ref="H48:L52"/>
@@ -5263,30 +5343,6 @@
     <mergeCell ref="B53:F57"/>
     <mergeCell ref="H53:L57"/>
     <mergeCell ref="N53:R57"/>
-    <mergeCell ref="B40:F43"/>
-    <mergeCell ref="H40:L43"/>
-    <mergeCell ref="N40:R43"/>
-    <mergeCell ref="B46:F47"/>
-    <mergeCell ref="H46:L47"/>
-    <mergeCell ref="N46:R47"/>
-    <mergeCell ref="B19:F23"/>
-    <mergeCell ref="H19:L23"/>
-    <mergeCell ref="N19:R23"/>
-    <mergeCell ref="B38:F39"/>
-    <mergeCell ref="H38:L39"/>
-    <mergeCell ref="N38:R39"/>
-    <mergeCell ref="B12:F13"/>
-    <mergeCell ref="H12:L13"/>
-    <mergeCell ref="N12:R13"/>
-    <mergeCell ref="B14:F18"/>
-    <mergeCell ref="H14:L18"/>
-    <mergeCell ref="N14:R18"/>
-    <mergeCell ref="B4:F5"/>
-    <mergeCell ref="H4:L5"/>
-    <mergeCell ref="N4:R5"/>
-    <mergeCell ref="B6:F9"/>
-    <mergeCell ref="H6:L9"/>
-    <mergeCell ref="N6:R9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>